<commit_message>
intregrate model to dashboard
</commit_message>
<xml_diff>
--- a/data/hotel_data.xlsx
+++ b/data/hotel_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AltoTech\weather\hotel_dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AltoTech\Hotel_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972C0242-932D-4F1A-A5EB-28EE6C896468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EB7514-B7EC-4220-8C08-23DEA156241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ชีต1" sheetId="1" r:id="rId1"/>
@@ -1126,8 +1126,8 @@
   </sheetPr>
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>